<commit_message>
Update flipkart buy product scenarios.xlsx
as
</commit_message>
<xml_diff>
--- a/assignment 2/flipkart buy product scenarios.xlsx
+++ b/assignment 2/flipkart buy product scenarios.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\2ND MODULE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Documents\GitHub\SAPNA-RAWAT\assignment 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E81401-3A5A-4FFA-AD2F-FAA0D900769E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCB8853-38F4-428C-971F-5313D1FD721F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="facebook" sheetId="1" r:id="rId1"/>
+    <sheet name="flipkart" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -135,7 +135,7 @@
     <t>sometimes the placed order gets cancelled automatically by the seller or flipkart.</t>
   </si>
   <si>
-    <t xml:space="preserve">                                                                  facebook</t>
+    <t xml:space="preserve">                                                                   flipcart</t>
   </si>
 </sst>
 </file>

</xml_diff>